<commit_message>
Relatorio semi-preenchido -> agora guardado :P
</commit_message>
<xml_diff>
--- a/Relatorio-DAD.xlsx
+++ b/Relatorio-DAD.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="D702" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
   <si>
     <t>Nº Grupo</t>
   </si>
@@ -451,6 +451,60 @@
   </si>
   <si>
     <t>Completo</t>
+  </si>
+  <si>
+    <t>Parcial</t>
+  </si>
+  <si>
+    <t>Falta enviar o mail de confirmação.</t>
+  </si>
+  <si>
+    <t>Tipo de aplicaçao: SPA; Tecnologias no cliente: Vue.js</t>
+  </si>
+  <si>
+    <t>São reactivos. Há comunicação entre o cliente e o servidor através dos sockets. E cada utilizador que esta ligado ao jogo consegue ver as alterções em tempo real, do(s) outro(s) jogador(es)</t>
+  </si>
+  <si>
+    <t>O looby é reactivo. Quando é criado um jogo aparece disponivel para outros jogadores online.</t>
+  </si>
+  <si>
+    <t>A aplicaçao está dividida nas sseguintes componentes: lobby.vue, login.vue, logout.vue, game-memory.vue, multiplayer_memory.vue, register.vue, single_player, user.vue, userEdit.vue</t>
+  </si>
+  <si>
+    <t>Sim, as rotas são: /login, /users, /singlememory, /multimemory; Usam navigation guards</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Sim, vue-moment, vue-router, vue-socket.io</t>
+  </si>
+  <si>
+    <t>Sim, usam middleware auth:api, que obriga a adicionar um header com autorizaçao + access_token</t>
+  </si>
+  <si>
+    <t>Na comunicação entre sockets garante-se que o servidor entrega dados no socket que está associado ao player</t>
+  </si>
+  <si>
+    <t>Não é mantido caso o Node falhe</t>
+  </si>
+  <si>
+    <t>Os jogos terminam tambem porque não é mantido o estado.</t>
+  </si>
+  <si>
+    <t>Não foram feitas optimizações</t>
+  </si>
+  <si>
+    <t>O board é construido com peças que "sabem" a sua posição, entao não é preciso enviar as coordenadas da peça clicada para o player, atraves do WebSocket</t>
+  </si>
+  <si>
+    <t>O player tem guardado o WebSocket id, a api tem middleware, as vue-routes têm navigation guards</t>
+  </si>
+  <si>
+    <t>Usamos os componentes do vue para optimizar o desempenho no cliente.</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -822,8 +876,48 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -837,51 +931,11 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1217,9 +1271,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1"/>
@@ -1342,417 +1396,452 @@
     </row>
     <row r="10" spans="2:9" ht="12" customHeight="1"/>
     <row r="11" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
     </row>
     <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
     </row>
     <row r="13" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="43"/>
     </row>
     <row r="14" spans="2:9" ht="11.1" customHeight="1">
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
     </row>
     <row r="15" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
     </row>
     <row r="16" spans="2:9" ht="65.099999999999994" customHeight="1">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="2:9" ht="135" customHeight="1">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="20" spans="2:9" ht="12" customHeight="1">
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
     </row>
     <row r="21" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="2:9" ht="134.1" customHeight="1">
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="2:9" ht="12" customHeight="1">
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
     </row>
     <row r="24" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
     </row>
     <row r="25" spans="2:9" ht="135.94999999999999" customHeight="1">
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="57"/>
     </row>
     <row r="26" spans="2:9" ht="12" customHeight="1">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
     </row>
     <row r="28" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="2:9" ht="137.1" customHeight="1">
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="45"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="57"/>
     </row>
     <row r="30" spans="2:9" ht="12" customHeight="1">
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
     </row>
     <row r="31" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
     </row>
     <row r="32" spans="2:9" ht="38.1" customHeight="1">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
     </row>
     <row r="33" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B33" s="58"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="55"/>
+      <c r="B33" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="43"/>
     </row>
     <row r="34" spans="2:9" ht="12" customHeight="1">
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
     </row>
     <row r="35" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
     </row>
     <row r="36" spans="2:9" ht="24" customHeight="1">
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
     </row>
     <row r="37" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="59"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="59" t="s">
+      <c r="E37" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
       <c r="I37" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="E38" s="58" t="s">
+      <c r="C38" s="43"/>
+      <c r="E38" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="54"/>
-      <c r="G38" s="55"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="43"/>
       <c r="H38" s="5"/>
       <c r="I38" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B39" s="58"/>
-      <c r="C39" s="55"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="55"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="43"/>
       <c r="H39" s="5"/>
       <c r="I39" s="40"/>
     </row>
     <row r="40" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B40" s="58"/>
-      <c r="C40" s="55"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="55"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="43"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="43"/>
       <c r="H40" s="5"/>
       <c r="I40" s="40"/>
     </row>
     <row r="41" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B41" s="58"/>
-      <c r="C41" s="55"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="55"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="43"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="43"/>
       <c r="H41" s="5"/>
       <c r="I41" s="40"/>
     </row>
     <row r="42" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B42" s="58"/>
-      <c r="C42" s="55"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="55"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="43"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="43"/>
       <c r="H42" s="5"/>
       <c r="I42" s="40"/>
     </row>
     <row r="43" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B43" s="58"/>
-      <c r="C43" s="55"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="55"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="43"/>
       <c r="H43" s="5"/>
       <c r="I43" s="40"/>
     </row>
     <row r="44" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B44" s="58"/>
-      <c r="C44" s="55"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="55"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="43"/>
       <c r="H44" s="5"/>
       <c r="I44" s="40"/>
     </row>
     <row r="45" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B45" s="58"/>
-      <c r="C45" s="55"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="55"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="43"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="43"/>
       <c r="H45" s="5"/>
       <c r="I45" s="40"/>
     </row>
     <row r="46" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B46" s="58"/>
-      <c r="C46" s="55"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="55"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="43"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="43"/>
       <c r="H46" s="5"/>
       <c r="I46" s="40"/>
     </row>
     <row r="47" spans="2:9" ht="21.95" customHeight="1">
-      <c r="B47" s="58"/>
-      <c r="C47" s="55"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="55"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="43"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="43"/>
       <c r="H47" s="5"/>
       <c r="I47" s="40"/>
     </row>
     <row r="49" spans="2:9" s="9" customFormat="1" ht="30.95" customHeight="1">
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
     </row>
   </sheetData>
   <sheetProtection password="D702" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="49">
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="E47:G47"/>
     <mergeCell ref="B37:C37"/>
@@ -1769,39 +1858,6 @@
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B49:I49"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I25"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD49">
     <cfRule type="expression" dxfId="2" priority="1">
@@ -1817,9 +1873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1874,9 +1930,11 @@
         <v>17</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="33"/>
+        <v>84</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>85</v>
+      </c>
       <c r="E6" s="22"/>
     </row>
     <row r="7" spans="2:9" s="23" customFormat="1" ht="68.099999999999994" customHeight="1">
@@ -1894,7 +1952,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="22"/>
@@ -1904,7 +1962,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="22"/>
@@ -1924,7 +1982,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="22"/>
@@ -1934,7 +1992,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="22"/>
@@ -1944,7 +2002,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="22"/>
@@ -2019,7 +2077,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D22" s="33"/>
       <c r="E22" s="22"/>
@@ -2049,7 +2107,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D25" s="33"/>
       <c r="E25" s="22"/>
@@ -2059,7 +2117,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="22"/>
@@ -2124,7 +2182,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="22"/>
@@ -2321,7 +2379,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -2368,133 +2426,171 @@
       <c r="B6" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>86</v>
+      </c>
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B7" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>86</v>
+      </c>
       <c r="D7" s="22"/>
     </row>
     <row r="8" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B8" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="33" t="s">
+        <v>87</v>
+      </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="33" t="s">
+        <v>88</v>
+      </c>
       <c r="D9" s="22"/>
     </row>
     <row r="10" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B10" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="33" t="s">
+        <v>89</v>
+      </c>
       <c r="D10" s="22"/>
     </row>
     <row r="11" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B11" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="33" t="s">
+        <v>90</v>
+      </c>
       <c r="D11" s="22"/>
     </row>
     <row r="12" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B12" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="33" t="s">
+        <v>91</v>
+      </c>
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B13" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33" t="s">
+        <v>92</v>
+      </c>
       <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B14" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="33" t="s">
+        <v>91</v>
+      </c>
       <c r="D14" s="22"/>
     </row>
     <row r="15" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B15" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="33" t="s">
+        <v>91</v>
+      </c>
       <c r="D15" s="22"/>
     </row>
     <row r="16" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B16" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="33" t="s">
+        <v>93</v>
+      </c>
       <c r="D16" s="22"/>
     </row>
     <row r="17" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B17" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="33" t="s">
+        <v>94</v>
+      </c>
       <c r="D17" s="22"/>
     </row>
     <row r="18" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B18" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="33" t="s">
+        <v>91</v>
+      </c>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="33" t="s">
+        <v>95</v>
+      </c>
       <c r="D19" s="22"/>
     </row>
     <row r="20" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B20" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="33" t="s">
+        <v>96</v>
+      </c>
       <c r="D20" s="22"/>
     </row>
     <row r="21" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B21" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="33" t="s">
+        <v>97</v>
+      </c>
       <c r="D21" s="22"/>
     </row>
     <row r="22" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="33" t="s">
+        <v>98</v>
+      </c>
       <c r="D22" s="22"/>
     </row>
     <row r="23" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B23" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="33" t="s">
+        <v>100</v>
+      </c>
       <c r="D23" s="22"/>
     </row>
     <row r="24" spans="2:8" s="23" customFormat="1" ht="75" customHeight="1">
       <c r="B24" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="33" t="s">
+        <v>99</v>
+      </c>
       <c r="D24" s="22"/>
     </row>
     <row r="25" spans="2:8" ht="26.25">

</xml_diff>